<commit_message>
add baseline to calculation
</commit_message>
<xml_diff>
--- a/excel_files/perceptualEval.xlsx
+++ b/excel_files/perceptualEval.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="152">
   <si>
     <t xml:space="preserve">submission_code</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t xml:space="preserve">DCASE2023_baseline_task7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline</t>
   </si>
   <si>
     <t xml:space="preserve">2.930</t>
@@ -753,10 +756,10 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="35.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="11.52"/>
@@ -1027,27 +1030,29 @@
       <c r="A10" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="C10" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1070,10 +1075,10 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1112,25 +1117,25 @@
         <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1141,25 +1146,25 @@
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,25 +1175,25 @@
         <v>28</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,25 +1204,25 @@
         <v>37</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1228,25 +1233,25 @@
         <v>46</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1257,25 +1262,25 @@
         <v>55</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,25 +1291,25 @@
         <v>63</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1315,52 +1320,54 @@
         <v>72</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="C10" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>